<commit_message>
end of day 3 update
</commit_message>
<xml_diff>
--- a/Tournament1Teams.xlsx
+++ b/Tournament1Teams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\Databse-Project-TBD\TheShowdownEffect.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A334B85-E36F-49E7-B609-E80EBEE4F34A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F112DAF9-DF34-4FB9-8164-8973513F5678}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="4800" windowWidth="25485" windowHeight="14595" xr2:uid="{CC34E7FB-F3C3-475C-A0A1-30CD59F5FA06}"/>
+    <workbookView xWindow="12210" yWindow="4275" windowWidth="25485" windowHeight="14595" xr2:uid="{CC34E7FB-F3C3-475C-A0A1-30CD59F5FA06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>Team</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>2 Bacon Nuggets</t>
+  </si>
+  <si>
+    <t>Substitute: Pookie</t>
+  </si>
+  <si>
+    <t>Substitute: Yante, Wrong Side of Average</t>
   </si>
 </sst>
 </file>
@@ -696,14 +702,14 @@
   <dimension ref="B3:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="A2" sqref="A2:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="4"/>
     <col min="2" max="2" width="18.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="33.25" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.125" style="4" customWidth="1"/>
     <col min="5" max="6" width="9" style="4"/>
     <col min="7" max="7" width="13.75" style="4" customWidth="1"/>
@@ -780,7 +786,7 @@
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D11" s="12"/>
     </row>
@@ -970,9 +976,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="9"/>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1032,12 +1040,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="D12:D15"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="B32:B35"/>
@@ -1048,6 +1050,12 @@
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="D24:D27"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="D12:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>